<commit_message>
Barema Seminário Sobre Microncontroladores Yduqs 31maio2023
</commit_message>
<xml_diff>
--- a/03 Assessments/notas AV1 microcontroladores projeto Arduino e MM.xlsx
+++ b/03 Assessments/notas AV1 microcontroladores projeto Arduino e MM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YduqsArea1\25 WydenArea1ProgramacaoMicrocontroladores\03 Assessments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9DB56E-8BF0-4E85-A099-0E49C31FA967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18951BDD-1DC3-465F-A3A0-EB33957772B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{37207522-E8FF-4681-8F81-32F57A53DE4E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Equipe</t>
   </si>
@@ -149,9 +149,6 @@
     <t>ED</t>
   </si>
   <si>
-    <t>Obs.: Aluno novo</t>
-  </si>
-  <si>
     <t>Obs.: Joaquim não fez o MM</t>
   </si>
   <si>
@@ -216,6 +213,12 @@
   </si>
   <si>
     <t>Obs: Resist mal definido, reconsiderei.</t>
+  </si>
+  <si>
+    <t>Obs.: Aluno novo; entregou atrasado - será dado a nota na AV3(Nota da AV1)</t>
+  </si>
+  <si>
+    <t>ALAN ROBERT SILVA BARROS</t>
   </si>
 </sst>
 </file>
@@ -698,10 +701,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AED4F9D-46A6-4463-AA32-0C4C94548B61}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,10 +733,10 @@
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5">
         <v>9</v>
@@ -760,10 +763,10 @@
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -772,7 +775,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
@@ -785,7 +788,7 @@
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="20" t="s">
         <v>6</v>
@@ -797,7 +800,7 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
@@ -818,7 +821,7 @@
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>21</v>
@@ -851,7 +854,7 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>7</v>
@@ -879,12 +882,12 @@
         <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="11" t="s">
         <v>13</v>
@@ -906,7 +909,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26">
         <v>8.5</v>
@@ -915,7 +918,7 @@
         <v>0</v>
       </c>
       <c r="G26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
@@ -951,12 +954,12 @@
         <v>1</v>
       </c>
       <c r="G30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>18</v>
@@ -972,7 +975,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>10</v>
@@ -984,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="G34" s="23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -994,7 +997,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D36" s="18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -1005,7 +1008,7 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D38" s="14" t="s">
         <v>12</v>
@@ -1022,7 +1025,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D40" s="22" t="s">
         <v>35</v>
@@ -1034,21 +1037,29 @@
         <v>0</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C42">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D41" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G41" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C43">
         <v>12</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="G43" t="s">
         <v>57</v>
-      </c>
-      <c r="E42">
-        <v>7</v>
-      </c>
-      <c r="G42" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>